<commit_message>
refactor: delete language entity
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="tags" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="notes" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="language_English" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="language_ENG" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="settings" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
@@ -160,7 +160,7 @@
     <t xml:space="preserve">vocabulary pagination</t>
   </si>
   <si>
-    <t xml:space="preserve">English</t>
+    <t xml:space="preserve">ENG</t>
   </si>
 </sst>
 </file>
@@ -170,7 +170,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -191,11 +191,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -240,16 +235,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -272,11 +263,11 @@
   </sheetPr>
   <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L9" activeCellId="0" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.78515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -330,9 +321,9 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.78515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="111.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="111.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="49.05"/>
   </cols>
@@ -363,7 +354,7 @@
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
@@ -372,7 +363,7 @@
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -599,7 +590,7 @@
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.78515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -727,10 +718,6 @@
       <c r="D9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
@@ -1196,11 +1183,11 @@
   </sheetPr>
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.78515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
feat: (vocabulary-service) add translations to vocabulary entry
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="tags" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="47">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t xml:space="preserve">contexts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">translations</t>
   </si>
   <si>
     <t xml:space="preserve">mediocre</t>
@@ -267,7 +270,7 @@
       <selection pane="topLeft" activeCell="L9" activeCellId="0" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -321,7 +324,7 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="111.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.45"/>
@@ -584,13 +587,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G85"/>
+  <dimension ref="A1:H85"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -614,95 +617,98 @@
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="H1" s="0" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>0</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>0</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1183,35 +1189,35 @@
   </sheetPr>
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>6</v>

</xml_diff>